<commit_message>
230212_excel file_reading and set values
</commit_message>
<xml_diff>
--- a/PlikDoOdczytu.xlsx
+++ b/PlikDoOdczytu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JAVA\221004_CurrencyExchangeApplication\CurrencyExchangeApplication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrzej\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF6E249-6A44-4502-A3A1-897DA7103A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A20B68A-EFDF-4F86-BF8E-2E23594086F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="15375" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="1980" windowWidth="15375" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Andrzej Wojciechowski" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>PLN</t>
   </si>
@@ -31,7 +31,19 @@
     <t>USD</t>
   </si>
   <si>
-    <t>tttext</t>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>DKK</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>amount</t>
   </si>
 </sst>
 </file>
@@ -67,9 +79,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -384,42 +401,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
         <v>1000</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>500</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>1250</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5">
-        <v>50</v>
+      <c r="E2" s="2">
+        <v>200</v>
+      </c>
+      <c r="F2" s="2">
+        <v>600</v>
+      </c>
+      <c r="G2" s="2">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
230213_excel file_reading and set values
</commit_message>
<xml_diff>
--- a/PlikDoOdczytu.xlsx
+++ b/PlikDoOdczytu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JAVA\221004_CurrencyExchangeApplication\CurrencyExchangeApplication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrzej\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF6E249-6A44-4502-A3A1-897DA7103A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A20B68A-EFDF-4F86-BF8E-2E23594086F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="15375" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="1980" windowWidth="15375" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Andrzej Wojciechowski" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>PLN</t>
   </si>
@@ -31,7 +31,19 @@
     <t>USD</t>
   </si>
   <si>
-    <t>tttext</t>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>DKK</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>amount</t>
   </si>
 </sst>
 </file>
@@ -67,9 +79,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -384,42 +401,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
         <v>1000</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>500</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>1250</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5">
-        <v>50</v>
+      <c r="E2" s="2">
+        <v>200</v>
+      </c>
+      <c r="F2" s="2">
+        <v>600</v>
+      </c>
+      <c r="G2" s="2">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>